<commit_message>
Working on Maine xslt.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Vehicle_Crash_Query_Results/artifacts/service_model/information_model/IEPD/documentation/VehicleCrashQueryResults-1.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Vehicle_Crash_Query_Results/artifacts/service_model/information_model/IEPD/documentation/VehicleCrashQueryResults-1.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="660" windowWidth="24560" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="4220" yWindow="540" windowWidth="24560" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicle Crash" sheetId="1" r:id="rId1"/>
-    <sheet name="Codes" sheetId="2" r:id="rId2"/>
+    <sheet name="Maine Codes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="278">
   <si>
     <t>Description</t>
   </si>
@@ -700,15 +700,9 @@
     <t>Person ID</t>
   </si>
   <si>
-    <t>Use Maine Code</t>
-  </si>
-  <si>
     <t>NIEM Code</t>
   </si>
   <si>
-    <t>Ude NIEM Code</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -848,6 +842,18 @@
   </si>
   <si>
     <t>CrashDriverLicenseCrash</t>
+  </si>
+  <si>
+    <t>Use NIEM Code</t>
+  </si>
+  <si>
+    <t>City or Town Code</t>
+  </si>
+  <si>
+    <t>Driver License Restriction Code</t>
+  </si>
+  <si>
+    <t>Use Maine Code (Red=As of 10/4/16)</t>
   </si>
 </sst>
 </file>
@@ -972,7 +978,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF6600"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -1316,7 +1321,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1392,6 +1397,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="236">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
@@ -1930,9 +1938,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G174"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84:XFD84"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2513,7 +2521,7 @@
     </row>
     <row r="58" spans="3:7" s="6" customFormat="1" ht="14" customHeight="1">
       <c r="C58" s="22" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="19"/>
@@ -2814,7 +2822,7 @@
     </row>
     <row r="89" spans="3:7" s="6" customFormat="1" ht="14" customHeight="1">
       <c r="C89" s="22" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
@@ -3613,36 +3621,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A81" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="40.6640625" style="20" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="59.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="37" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="C1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E1" t="s">
-        <v>247</v>
+      <c r="D1" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3659,8 +3667,8 @@
       <c r="A4" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="B4" t="s">
-        <v>229</v>
+      <c r="B4" s="25" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3675,236 +3683,277 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" t="s">
-        <v>229</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B8" t="s">
-        <v>229</v>
-      </c>
+      <c r="B8" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="B9" t="s">
-        <v>229</v>
-      </c>
+      <c r="B9" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B10" t="s">
-        <v>229</v>
-      </c>
+      <c r="B10" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
-        <v>229</v>
-      </c>
+      <c r="B11" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
-        <v>229</v>
-      </c>
+      <c r="B12" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C13" t="s">
-        <v>229</v>
-      </c>
-      <c r="E13" t="s">
-        <v>240</v>
+      <c r="B13" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C14" t="s">
-        <v>229</v>
-      </c>
-      <c r="E14" t="s">
-        <v>241</v>
+      <c r="B14" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C15" t="s">
-        <v>229</v>
-      </c>
-      <c r="E15" t="s">
-        <v>242</v>
+      <c r="B15" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C16" t="s">
-        <v>229</v>
-      </c>
-      <c r="E16" t="s">
-        <v>243</v>
+      <c r="B16" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C17" t="s">
-        <v>229</v>
-      </c>
-      <c r="E17" t="s">
-        <v>244</v>
+      <c r="B17" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B18" t="s">
-        <v>229</v>
-      </c>
+      <c r="B18" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C19" t="s">
-        <v>229</v>
-      </c>
-      <c r="E19" t="s">
-        <v>239</v>
+      <c r="B19" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C20" t="s">
-        <v>229</v>
-      </c>
-      <c r="E20" t="s">
-        <v>245</v>
+      <c r="B20" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C21" t="s">
-        <v>229</v>
-      </c>
-      <c r="E21" t="s">
-        <v>233</v>
+      <c r="B21" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C22" t="s">
-        <v>229</v>
-      </c>
-      <c r="E22" t="s">
-        <v>246</v>
+      <c r="B22" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="B23" t="s">
-        <v>229</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="B24" t="s">
-        <v>229</v>
-      </c>
+      <c r="B24" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B25" t="s">
-        <v>229</v>
-      </c>
+      <c r="B25" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B26" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E26" t="s">
-        <v>248</v>
+      <c r="B26" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B27" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D27" t="s">
-        <v>229</v>
-      </c>
-      <c r="E27" t="s">
-        <v>249</v>
+      <c r="B27" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3912,13 +3961,14 @@
         <v>188</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D28" t="s">
-        <v>229</v>
-      </c>
-      <c r="E28" t="s">
-        <v>250</v>
+        <v>227</v>
+      </c>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3926,178 +3976,209 @@
         <v>57</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D29" t="s">
-        <v>229</v>
-      </c>
-      <c r="E29" t="s">
-        <v>251</v>
+        <v>227</v>
+      </c>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B30" t="s">
-        <v>229</v>
-      </c>
+      <c r="B30" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C31" t="s">
-        <v>229</v>
-      </c>
-      <c r="E31" t="s">
-        <v>252</v>
+      <c r="B31" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B32" t="s">
-        <v>229</v>
-      </c>
+      <c r="B32" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B33" t="s">
-        <v>229</v>
-      </c>
+      <c r="B33" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B34" t="s">
-        <v>229</v>
-      </c>
-      <c r="E34" t="s">
-        <v>253</v>
+      <c r="B34" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C35" t="s">
-        <v>229</v>
-      </c>
-      <c r="E35" t="s">
-        <v>234</v>
+      <c r="B35" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="B36" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D36" t="s">
-        <v>229</v>
-      </c>
-      <c r="E36" t="s">
-        <v>254</v>
+      <c r="B36" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="B37" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C37" t="s">
-        <v>229</v>
-      </c>
-      <c r="E37" t="s">
-        <v>255</v>
+      <c r="B37" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="B38" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D38" t="s">
-        <v>229</v>
-      </c>
-      <c r="E38" t="s">
-        <v>237</v>
+      <c r="B38" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B39" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C39" t="s">
-        <v>229</v>
-      </c>
-      <c r="E39" t="s">
-        <v>256</v>
+      <c r="B39" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B40" t="s">
-        <v>229</v>
-      </c>
+      <c r="B40" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B41" t="s">
-        <v>229</v>
-      </c>
+      <c r="B41" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B43" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C43" t="s">
-        <v>229</v>
-      </c>
+      <c r="B43" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="5" t="s">
         <v>196</v>
       </c>
       <c r="B44" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26" t="s">
         <v>229</v>
-      </c>
-      <c r="C44" t="s">
-        <v>229</v>
-      </c>
-      <c r="E44" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -4105,109 +4186,129 @@
         <v>195</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C45" t="s">
-        <v>229</v>
-      </c>
-      <c r="E45" t="s">
-        <v>257</v>
+        <v>227</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C46" t="s">
-        <v>229</v>
-      </c>
-      <c r="E46" t="s">
-        <v>230</v>
+      <c r="B46" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B47" t="s">
-        <v>229</v>
-      </c>
+      <c r="B47" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B48" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C48" t="s">
-        <v>229</v>
-      </c>
-      <c r="E48" t="s">
-        <v>258</v>
+      <c r="B48" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B49" t="s">
-        <v>229</v>
-      </c>
+      <c r="B49" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B50" t="s">
-        <v>229</v>
-      </c>
+      <c r="B50" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B51" t="s">
-        <v>229</v>
-      </c>
-      <c r="E51" t="s">
-        <v>236</v>
+      <c r="B51" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B52" t="s">
-        <v>229</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B53" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="E53" t="s">
-        <v>262</v>
+      <c r="B53" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C54" t="s">
-        <v>229</v>
-      </c>
-      <c r="E54" t="s">
-        <v>259</v>
+      <c r="B54" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -4215,126 +4316,163 @@
         <v>62</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C55" t="s">
-        <v>229</v>
-      </c>
-      <c r="E55" t="s">
-        <v>261</v>
+        <v>227</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B56" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C56" t="s">
-        <v>229</v>
-      </c>
-      <c r="E56" t="s">
-        <v>260</v>
+      <c r="B56" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="4" t="s">
         <v>213</v>
       </c>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="5" t="s">
         <v>173</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>229</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B61" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C61" t="s">
-        <v>229</v>
-      </c>
+      <c r="B61" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="4" t="s">
         <v>214</v>
       </c>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B64" t="s">
-        <v>229</v>
-      </c>
+      <c r="B64" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B65" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D65" t="s">
-        <v>229</v>
-      </c>
+      <c r="B65" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E65" s="26"/>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B66" s="25" t="s">
-        <v>229</v>
-      </c>
+      <c r="B66" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B67" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D67" t="s">
-        <v>229</v>
-      </c>
-      <c r="E67" t="s">
-        <v>264</v>
+      <c r="B67" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C67" s="26"/>
+      <c r="D67" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E67" s="26" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="B68" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D68" t="s">
-        <v>229</v>
-      </c>
-      <c r="E68" t="s">
-        <v>263</v>
+      <c r="B68" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E68" s="26" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -4342,27 +4480,29 @@
         <v>88</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C69" t="s">
-        <v>229</v>
-      </c>
-      <c r="E69" t="s">
-        <v>266</v>
+        <v>227</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="9" t="s">
+      <c r="A70" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B70" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C70" t="s">
-        <v>229</v>
-      </c>
-      <c r="E70" t="s">
-        <v>265</v>
+      <c r="B70" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C70" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -4370,13 +4510,14 @@
         <v>90</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C71" t="s">
-        <v>229</v>
-      </c>
-      <c r="E71" t="s">
-        <v>267</v>
+        <v>227</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -4384,187 +4525,245 @@
         <v>91</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C72" t="s">
-        <v>229</v>
-      </c>
-      <c r="E72" t="s">
-        <v>268</v>
+        <v>227</v>
+      </c>
+      <c r="C72" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B73" t="s">
-        <v>229</v>
-      </c>
+      <c r="B73" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B74" t="s">
-        <v>229</v>
-      </c>
+      <c r="B74" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B75" t="s">
-        <v>229</v>
-      </c>
+      <c r="B75" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="20" t="s">
         <v>95</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C76" t="s">
-        <v>229</v>
-      </c>
-      <c r="E76" t="s">
-        <v>238</v>
+        <v>227</v>
+      </c>
+      <c r="C76" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B77" t="s">
-        <v>229</v>
-      </c>
+      <c r="B77" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C77" s="26"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="26"/>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B78" t="s">
-        <v>229</v>
-      </c>
+      <c r="B78" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
+      <c r="E78" s="26"/>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B79" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C79" t="s">
-        <v>229</v>
-      </c>
-      <c r="E79" t="s">
-        <v>269</v>
+      <c r="B79" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C79" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D79" s="26"/>
+      <c r="E79" s="26" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B80" t="s">
-        <v>229</v>
-      </c>
+      <c r="B80" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C80" s="26"/>
+      <c r="D80" s="26"/>
+      <c r="E80" s="26"/>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B81" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C81" t="s">
-        <v>229</v>
-      </c>
-      <c r="E81" t="s">
-        <v>270</v>
+      <c r="B81" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C81" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B82" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C82" t="s">
-        <v>229</v>
-      </c>
-      <c r="E82" t="s">
-        <v>271</v>
+      <c r="B82" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C82" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="B83" s="26"/>
+      <c r="C83" s="26"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="26"/>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="5" t="s">
         <v>193</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>229</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="C84" s="26"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B85" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C85" t="s">
-        <v>229</v>
-      </c>
-      <c r="E85" t="s">
-        <v>272</v>
+      <c r="B85" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C85" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B86" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C86" t="s">
-        <v>229</v>
-      </c>
-      <c r="E86" t="s">
-        <v>275</v>
+      <c r="B86" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C86" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B87" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C87" t="s">
-        <v>229</v>
-      </c>
-      <c r="E87" t="s">
-        <v>274</v>
+      <c r="B87" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C87" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D87" s="26"/>
+      <c r="E87" s="26" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B88" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C88" t="s">
-        <v>229</v>
-      </c>
-      <c r="E88" t="s">
-        <v>273</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="B88" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C88" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D88" s="26"/>
+      <c r="E88" s="26" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="B89" s="26"/>
+      <c r="C89" s="26"/>
+      <c r="D89" s="26"/>
+      <c r="E89" s="26"/>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="B90" s="26"/>
+      <c r="C90" s="26"/>
+      <c r="D90" s="26"/>
+      <c r="E90" s="26"/>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="B91" s="26"/>
+      <c r="C91" s="26"/>
+      <c r="D91" s="26"/>
+      <c r="E91" s="26"/>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="B92" s="26"/>
+      <c r="C92" s="26"/>
+      <c r="D92" s="26"/>
+      <c r="E92" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>